<commit_message>
Update WorldScape system: multi-crop support, calibration improvements, and UI enhancements
- Add support for 5 crops: cotton, coffee, chili, garlic, onion
- Implement coffee calibration and isoscape generation
- Add risk mitigation dashboard with scenario analysis
- Improve interactive maps with overlays and styling
- Update calibration workflows and validation tools
- Add comprehensive documentation and status reports
</commit_message>
<xml_diff>
--- a/FTMapping/input/inline_samples.xlsx
+++ b/FTMapping/input/inline_samples.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -372,11 +372,31 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>OLD01</t>
+          <t>157</t>
         </is>
       </c>
       <c r="B2">
-        <v>30</v>
+        <v>31.1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>158</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>30.2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>159</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>29.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>